<commit_message>
phase 2 of resource game
</commit_message>
<xml_diff>
--- a/test_initial_states/game_initial_state.xlsx
+++ b/test_initial_states/game_initial_state.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Desktop/Class Material/CS 4269/ai_project/test_initial_states/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B04D0B7-38CE-D142-BA94-BDBE91EC78BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACA5DF7-3D01-1E48-8809-E89CD45FE14F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{65B8699D-C102-4177-9EDB-4160093663D6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{65B8699D-C102-4177-9EDB-4160093663D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -499,7 +499,7 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -665,8 +665,8 @@
       <c r="F3" s="2">
         <v>5000</v>
       </c>
-      <c r="G3" s="2">
-        <v>400</v>
+      <c r="G3" s="6">
+        <v>50000</v>
       </c>
       <c r="H3" s="6">
         <v>50000</v>
@@ -736,8 +736,8 @@
       <c r="F4" s="2">
         <v>1250</v>
       </c>
-      <c r="G4" s="2">
-        <v>200</v>
+      <c r="G4" s="5">
+        <v>5000</v>
       </c>
       <c r="H4" s="2">
         <v>7500</v>
@@ -807,8 +807,8 @@
       <c r="F5" s="5">
         <v>250</v>
       </c>
-      <c r="G5" s="1">
-        <v>100</v>
+      <c r="G5" s="4">
+        <v>6000</v>
       </c>
       <c r="H5" s="1">
         <v>17500</v>
@@ -879,7 +879,7 @@
         <v>4000</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="H6" s="4">
         <v>5000</v>

</xml_diff>